<commit_message>
CV ready to publish
</commit_message>
<xml_diff>
--- a/data/pubs.xlsx
+++ b/data/pubs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/Resume/wright_cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6835ABA4-EDB0-324B-9A19-66F4A39B6B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4787B17B-CBBA-5D46-A2B6-20F533740084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15660" xr2:uid="{9F01FDA3-1E1B-6547-B661-3F940585A8E2}"/>
   </bookViews>
@@ -156,12 +156,6 @@
     <t>Identifying Key Treatment Ingredients SLPs Utilize to Treat Persistent Cognitive Symptoms Post-Concussion in Adolescents</t>
   </si>
   <si>
-    <t xml:space="preserve">Center on Brain Injury Research and Training Webinar </t>
-  </si>
-  <si>
-    <t xml:space="preserve">webinar </t>
-  </si>
-  <si>
     <t>Eugene, OR</t>
   </si>
   <si>
@@ -181,6 +175,12 @@
   </si>
   <si>
     <t>https://doi.org/10.1097/TLD.0000000000000198</t>
+  </si>
+  <si>
+    <t>Center on Brain Injury Research and Training</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Webinar </t>
   </si>
 </sst>
 </file>
@@ -540,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AD3C43B-6729-8048-9A95-5F6194EDFE7F}">
   <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="L3" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -674,7 +674,7 @@
         <v>20</v>
       </c>
       <c r="J3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>23</v>
@@ -697,13 +697,13 @@
         <v>37</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="O4" s="1" t="b">
         <v>0</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="Q4" s="1" t="b">
         <v>0</v>
@@ -726,13 +726,13 @@
         <v>38</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="O5" s="1" t="b">
         <v>0</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q5" s="1" t="b">
         <v>1</v>
@@ -755,13 +755,13 @@
         <v>39</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="O6" s="1" t="b">
         <v>0</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q6" s="1" t="b">
         <v>1</v>
@@ -784,13 +784,13 @@
         <v>37</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O7" s="1" t="b">
         <v>0</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="Q7" s="1" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
CV update 8.24.21 ready to share
</commit_message>
<xml_diff>
--- a/data/pubs.xlsx
+++ b/data/pubs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/Resume/wright_cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864B44D0-058C-0345-91B5-1169FFD6D87F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9191A52A-74AD-D749-B447-CF16BDDD95E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-17900" yWindow="-19080" windowWidth="27640" windowHeight="15660" xr2:uid="{9F01FDA3-1E1B-6547-B661-3F940585A8E2}"/>
   </bookViews>
@@ -597,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AD3C43B-6729-8048-9A95-5F6194EDFE7F}">
   <dimension ref="A1:W11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D5" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="M8" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -951,7 +951,7 @@
         <v>52</v>
       </c>
       <c r="Q11" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R11" s="1" t="s">
         <v>53</v>

</xml_diff>

<commit_message>
dissertation pub added to CV
</commit_message>
<xml_diff>
--- a/data/pubs.xlsx
+++ b/data/pubs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/Resume/wright_cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9191A52A-74AD-D749-B447-CF16BDDD95E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DDEF984-5052-4044-BEE3-F7941133F1CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-17900" yWindow="-19080" windowWidth="27640" windowHeight="15660" xr2:uid="{9F01FDA3-1E1B-6547-B661-3F940585A8E2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="66">
   <si>
     <t>type</t>
   </si>
@@ -204,9 +204,6 @@
     <t>Wright, J., Sohlberg, M.M., McIntosh, K., Seeley, J., Hadley, W., Blitz, D. &amp; Lowham, E.</t>
   </si>
   <si>
-    <t>What is the effect of personalized cognitive strategy instruction on facilitating return-to-learn for individuals experiencing prolonged concussion symptoms?</t>
-  </si>
-  <si>
     <t>submission</t>
   </si>
   <si>
@@ -225,19 +222,16 @@
     <t xml:space="preserve">"RULE"-ing out comprehension deficits: Validity of the RULE tool as a screener for measuring postsecondary reading comprehension </t>
   </si>
   <si>
-    <t>in_progress</t>
-  </si>
-  <si>
-    <t>Wright, J., Furutani, T., Sohlberg, M.M., Mashima, P., &amp; Murata, N.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A retrospective review of thirteen years of concussion symptom reporting and trajectory data across the State of Hawaii and its influence on the future of return-to-learn </t>
-  </si>
-  <si>
-    <t>[Unpublished manuscript]</t>
-  </si>
-  <si>
-    <t>Department of Communication Disorders &amp; Scienes, University of Oregon; Department of Kinesiology and Rehabilitation Sciences, University of Hawaii at Manoa; Department of Communication Sciences and Disorders, University of Hawaii at Manoa</t>
+    <t xml:space="preserve">Neuropsychological Rehabilitation </t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1080/09602011.2022.2074467</t>
+  </si>
+  <si>
+    <t>https://www.tandfonline.com/doi/full/10.1080/09602011.2022.2074467</t>
+  </si>
+  <si>
+    <t>What is the effect of personalized cognitive strategy instruction on facilitating return-to-learn for individuals experiencing prolonged concussion symptoms</t>
   </si>
 </sst>
 </file>
@@ -595,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AD3C43B-6729-8048-9A95-5F6194EDFE7F}">
-  <dimension ref="A1:W11"/>
+  <dimension ref="A1:W10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M8" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -643,10 +637,10 @@
         <v>11</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>24</v>
@@ -679,92 +673,97 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="102" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" ht="119" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2022</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="102" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D3" s="1">
         <v>2021</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="170" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:23" ht="170" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B4" s="1">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D4" s="1">
         <v>2020</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G4" s="1">
         <v>40</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H4" s="1">
         <v>1</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J4" t="s">
         <v>46</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" ht="119" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D4" s="1">
-        <v>2021</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="J4"/>
-      <c r="L4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:23" ht="119" x14ac:dyDescent="0.2">
@@ -775,52 +774,57 @@
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D5" s="1">
         <v>2021</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J5"/>
       <c r="L5" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="221" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" ht="136" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D6" s="1">
-        <v>2021</v>
+        <v>14</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J6"/>
-      <c r="L6" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>67</v>
+        <v>37</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="S6" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="136" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" ht="119" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>14</v>
@@ -829,19 +833,19 @@
         <v>34</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="Q7" s="1" t="b">
         <v>0</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="S7" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:23" ht="119" x14ac:dyDescent="0.2">
@@ -849,114 +853,85 @@
         <v>26</v>
       </c>
       <c r="B8" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="Q8" s="1" t="b">
         <v>0</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="S8" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="119" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" ht="136" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Q9" s="1" t="b">
         <v>0</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="S9" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="136" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="Q10" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="S10" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" ht="51" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="1">
-        <v>5</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q11" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="R11" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="S11" s="1" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
page numbers for published dissertation
</commit_message>
<xml_diff>
--- a/data/pubs.xlsx
+++ b/data/pubs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/Resume/wright_cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DDEF984-5052-4044-BEE3-F7941133F1CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFBAA183-2189-2745-A02A-F80D88693090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-17900" yWindow="-19080" windowWidth="27640" windowHeight="15660" xr2:uid="{9F01FDA3-1E1B-6547-B661-3F940585A8E2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="67">
   <si>
     <t>type</t>
   </si>
@@ -232,6 +232,9 @@
   </si>
   <si>
     <t>What is the effect of personalized cognitive strategy instruction on facilitating return-to-learn for individuals experiencing prolonged concussion symptoms</t>
+  </si>
+  <si>
+    <t>1-30</t>
   </si>
 </sst>
 </file>
@@ -591,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AD3C43B-6729-8048-9A95-5F6194EDFE7F}">
   <dimension ref="A1:W10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -692,6 +695,9 @@
       <c r="F2" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="I2" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="J2" s="1" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
October 2022 CBIRT presentation added
</commit_message>
<xml_diff>
--- a/data/pubs.xlsx
+++ b/data/pubs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/Resume/wright_cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFBAA183-2189-2745-A02A-F80D88693090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F61DBB-3EDC-E44A-83DC-4729F255B1BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17900" yWindow="-19080" windowWidth="27640" windowHeight="15660" xr2:uid="{9F01FDA3-1E1B-6547-B661-3F940585A8E2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16320" xr2:uid="{9F01FDA3-1E1B-6547-B661-3F940585A8E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="70">
   <si>
     <t>type</t>
   </si>
@@ -235,6 +235,15 @@
   </si>
   <si>
     <t>1-30</t>
+  </si>
+  <si>
+    <t>Wright, J.</t>
+  </si>
+  <si>
+    <t>2022, October</t>
+  </si>
+  <si>
+    <t>Translating Executive Functioning Challenges into Treatment Implementation to Support Return-to-Learn in the mTBI Population</t>
   </si>
 </sst>
 </file>
@@ -592,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AD3C43B-6729-8048-9A95-5F6194EDFE7F}">
-  <dimension ref="A1:W10"/>
+  <dimension ref="A1:W11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6:S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -796,7 +805,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="136" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" ht="119" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
@@ -804,14 +813,15 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>37</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="J6"/>
       <c r="P6" s="1" t="s">
         <v>47</v>
       </c>
@@ -825,7 +835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="119" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" ht="136" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -839,19 +849,19 @@
         <v>34</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="Q7" s="1" t="b">
         <v>0</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="S7" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:23" ht="119" x14ac:dyDescent="0.2">
@@ -865,25 +875,25 @@
         <v>14</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q8" s="1" t="b">
         <v>0</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="S8" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="136" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" ht="119" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
@@ -894,25 +904,25 @@
         <v>14</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q9" s="1" t="b">
         <v>0</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="S9" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" ht="136" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -920,24 +930,53 @@
         <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q10" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="S10" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="1">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="P10" s="1" t="s">
+      <c r="P11" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="Q10" s="1" t="b">
+      <c r="Q11" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="R10" s="1" t="s">
+      <c r="R11" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="S10" s="1" t="b">
+      <c r="S11" s="1" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
wy act report added
</commit_message>
<xml_diff>
--- a/data/pubs.xlsx
+++ b/data/pubs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/Resume/wright_cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0865FB-5570-A045-AD56-5E3D17CC8A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4532A3F2-56BE-DA4F-A597-32784E4AC507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16320" xr2:uid="{9F01FDA3-1E1B-6547-B661-3F940585A8E2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="82">
   <si>
     <t>type</t>
   </si>
@@ -274,6 +274,12 @@
   </si>
   <si>
     <t xml:space="preserve">Cherasaro, T. &amp; Wright, J. </t>
+  </si>
+  <si>
+    <t>Scott, C., Wolfe, C., Rice, D., &amp; Wright, J.</t>
+  </si>
+  <si>
+    <t>Wyoming Accountability Part 1: An examination of the current system</t>
   </si>
 </sst>
 </file>
@@ -631,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AD3C43B-6729-8048-9A95-5F6194EDFE7F}">
-  <dimension ref="A1:W15"/>
+  <dimension ref="A1:W16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -752,7 +758,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>14</v>
@@ -781,7 +787,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>15</v>
@@ -1010,7 +1016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="102" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" ht="68" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>70</v>
       </c>
@@ -1018,13 +1024,13 @@
         <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D12" s="1">
         <v>2023</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>72</v>
@@ -1038,19 +1044,19 @@
         <v>2</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D13" s="1">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" ht="102" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>70</v>
       </c>
@@ -1058,19 +1064,19 @@
         <v>3</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D14" s="1">
         <v>2022</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="102" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>70</v>
       </c>
@@ -1078,15 +1084,35 @@
         <v>4</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D15" s="1">
         <v>2022</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="102" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="1">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="1">
+        <v>2022</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Summer 2024 Updates with CBIRT presentation
</commit_message>
<xml_diff>
--- a/data/pubs.xlsx
+++ b/data/pubs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/Resume/wright_cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9863F98-9DB2-3C45-B266-69037D4E46D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50ABD4C4-0CB0-C148-AF3F-45B8D4DE4CFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12620" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{9F01FDA3-1E1B-6547-B661-3F940585A8E2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="84">
   <si>
     <t>type</t>
   </si>
@@ -198,30 +198,18 @@
     <t>Rosemont, IL</t>
   </si>
   <si>
-    <t>under_review</t>
-  </si>
-  <si>
     <t>Wright, J., Sohlberg, M.M., McIntosh, K., Seeley, J., Hadley, W., Blitz, D. &amp; Lowham, E.</t>
   </si>
   <si>
     <t>submission</t>
   </si>
   <si>
-    <t>[Manuscript submitted for publication]</t>
-  </si>
-  <si>
     <t>department</t>
   </si>
   <si>
     <t>Department of Communication Disorders &amp; Sciences, University of Oregon</t>
   </si>
   <si>
-    <t>Kucheria, P., Sohlberg, M.M., Fickas, S. Prideaux, J., &amp; Wright, J.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"RULE"-ing out comprehension deficits: Validity of the RULE tool as a screener for measuring postsecondary reading comprehension </t>
-  </si>
-  <si>
     <t xml:space="preserve">Neuropsychological Rehabilitation </t>
   </si>
   <si>
@@ -292,6 +280,12 @@
   </si>
   <si>
     <t>Re-Imagining Remote Education in South Dakota: The ESF-REM Project; Final evaluation report</t>
+  </si>
+  <si>
+    <t>2024, May</t>
+  </si>
+  <si>
+    <t>Multidisciplinary Coordination and Communication to Guide Concussion Recovery</t>
   </si>
 </sst>
 </file>
@@ -353,9 +347,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -393,7 +387,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -499,7 +493,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -641,7 +635,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -651,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AD3C43B-6729-8048-9A95-5F6194EDFE7F}">
   <dimension ref="A1:W18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -697,10 +691,10 @@
         <v>11</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>24</v>
@@ -741,28 +735,28 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" s="1">
         <v>2022</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="J2" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="102" x14ac:dyDescent="0.2">
@@ -829,28 +823,34 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="119" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" ht="85" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="1">
-        <v>2021</v>
+        <v>63</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="J5"/>
-      <c r="L5" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>59</v>
+      <c r="P5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="S5" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="119" x14ac:dyDescent="0.2">
@@ -858,16 +858,16 @@
         <v>26</v>
       </c>
       <c r="B6" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J6"/>
       <c r="P6" s="1" t="s">
@@ -888,7 +888,7 @@
         <v>26</v>
       </c>
       <c r="B7" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>14</v>
@@ -917,7 +917,7 @@
         <v>26</v>
       </c>
       <c r="B8" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>14</v>
@@ -946,7 +946,7 @@
         <v>26</v>
       </c>
       <c r="B9" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>14</v>
@@ -975,7 +975,7 @@
         <v>26</v>
       </c>
       <c r="B10" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>14</v>
@@ -1004,7 +1004,7 @@
         <v>26</v>
       </c>
       <c r="B11" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>49</v>
@@ -1030,142 +1030,142 @@
     </row>
     <row r="12" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D12" s="1">
         <v>2023</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:23" ht="85" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B13" s="1">
         <v>2</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D13" s="1">
         <v>2023</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:23" ht="68" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B14" s="1">
         <v>3</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D14" s="1">
         <v>2023</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:23" ht="102" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B15" s="1">
         <v>4</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D15" s="1">
         <v>2023</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:23" ht="102" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B16" s="1">
         <v>5</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D16" s="1">
         <v>2022</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B17" s="1">
         <v>6</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D17" s="1">
         <v>2022</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B18" s="1">
         <v>7</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D18" s="1">
         <v>2022</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>